<commit_message>
update create content excel
</commit_message>
<xml_diff>
--- a/contentexcel/full_content_excel.xlsx
+++ b/contentexcel/full_content_excel.xlsx
@@ -270,9 +270,6 @@
     <t>Operator 17 / Stc Kuw</t>
   </si>
   <si>
-    <t>Operator18 / Vodafone Eg</t>
-  </si>
-  <si>
     <t>Operator 19 / Zain Bahrain</t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>IVAS</t>
+  </si>
+  <si>
+    <t>Operator 18 / Vodafone Eg</t>
   </si>
 </sst>
 </file>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AL1" sqref="AL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,54 +863,54 @@
         <v>36</v>
       </c>
       <c r="AL1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="AZ1" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:52" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="T2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove colums from excel
</commit_message>
<xml_diff>
--- a/contentexcel/full_content_excel.xlsx
+++ b/contentexcel/full_content_excel.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BC$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AY$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -56,84 +56,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>mohamed mahmoud:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-2020-10-22</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>mohamed mahmoud:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-2020-10-22</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>mohamed mahmoud:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-2020-10-22</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Occasion</t>
   </si>
@@ -171,22 +99,10 @@
     <t>Content Path</t>
   </si>
   <si>
-    <t>Content Start Date</t>
-  </si>
-  <si>
-    <t>Content Expire Date</t>
-  </si>
-  <si>
     <t>Rbt Name En</t>
   </si>
   <si>
     <t>Rbt Name Ar</t>
-  </si>
-  <si>
-    <t>RBT Start Date</t>
-  </si>
-  <si>
-    <t>RBT Expire Date</t>
   </si>
   <si>
     <t>Aggregator</t>
@@ -386,13 +302,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
@@ -677,7 +590,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC2"/>
+  <dimension ref="A1:AY2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -697,45 +610,41 @@
     <col min="11" max="11" width="33.85546875" customWidth="1"/>
     <col min="12" max="12" width="34" customWidth="1"/>
     <col min="13" max="15" width="33.7109375" customWidth="1"/>
-    <col min="16" max="16" width="27.5703125" customWidth="1"/>
-    <col min="17" max="17" width="27.85546875" customWidth="1"/>
-    <col min="18" max="19" width="54.140625" customWidth="1"/>
-    <col min="20" max="20" width="22.5703125" customWidth="1"/>
-    <col min="21" max="21" width="19.28515625" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" style="3" customWidth="1"/>
-    <col min="23" max="23" width="15.85546875" customWidth="1"/>
-    <col min="24" max="24" width="26.28515625" customWidth="1"/>
-    <col min="25" max="25" width="26.7109375" customWidth="1"/>
-    <col min="26" max="26" width="24.85546875" customWidth="1"/>
-    <col min="27" max="27" width="26.5703125" customWidth="1"/>
-    <col min="28" max="28" width="23" customWidth="1"/>
-    <col min="29" max="29" width="27.42578125" customWidth="1"/>
-    <col min="30" max="30" width="26.7109375" customWidth="1"/>
-    <col min="31" max="31" width="24" customWidth="1"/>
-    <col min="32" max="32" width="27.140625" customWidth="1"/>
-    <col min="33" max="33" width="30.28515625" customWidth="1"/>
-    <col min="34" max="34" width="26" customWidth="1"/>
-    <col min="35" max="35" width="27" customWidth="1"/>
-    <col min="36" max="36" width="27.28515625" customWidth="1"/>
-    <col min="37" max="37" width="27.42578125" customWidth="1"/>
-    <col min="38" max="38" width="27.5703125" customWidth="1"/>
-    <col min="39" max="40" width="27.42578125" customWidth="1"/>
-    <col min="41" max="41" width="27.85546875" customWidth="1"/>
-    <col min="42" max="42" width="27.7109375" customWidth="1"/>
-    <col min="43" max="43" width="27.85546875" customWidth="1"/>
-    <col min="44" max="44" width="27.28515625" customWidth="1"/>
-    <col min="45" max="45" width="27.5703125" customWidth="1"/>
+    <col min="16" max="17" width="54.140625" customWidth="1"/>
+    <col min="18" max="18" width="22.5703125" customWidth="1"/>
+    <col min="19" max="19" width="15.85546875" customWidth="1"/>
+    <col min="20" max="20" width="26.28515625" customWidth="1"/>
+    <col min="21" max="21" width="26.7109375" customWidth="1"/>
+    <col min="22" max="22" width="24.85546875" customWidth="1"/>
+    <col min="23" max="23" width="26.5703125" customWidth="1"/>
+    <col min="24" max="24" width="23" customWidth="1"/>
+    <col min="25" max="25" width="27.42578125" customWidth="1"/>
+    <col min="26" max="26" width="26.7109375" customWidth="1"/>
+    <col min="27" max="27" width="24" customWidth="1"/>
+    <col min="28" max="28" width="27.140625" customWidth="1"/>
+    <col min="29" max="29" width="30.28515625" customWidth="1"/>
+    <col min="30" max="30" width="26" customWidth="1"/>
+    <col min="31" max="31" width="27" customWidth="1"/>
+    <col min="32" max="32" width="27.28515625" customWidth="1"/>
+    <col min="33" max="33" width="27.42578125" customWidth="1"/>
+    <col min="34" max="34" width="27.5703125" customWidth="1"/>
+    <col min="35" max="36" width="27.42578125" customWidth="1"/>
+    <col min="37" max="37" width="27.85546875" customWidth="1"/>
+    <col min="38" max="38" width="27.7109375" customWidth="1"/>
+    <col min="39" max="39" width="27.85546875" customWidth="1"/>
+    <col min="40" max="40" width="27.28515625" customWidth="1"/>
+    <col min="41" max="41" width="27.5703125" customWidth="1"/>
+    <col min="42" max="43" width="28" customWidth="1"/>
+    <col min="44" max="44" width="27.85546875" customWidth="1"/>
+    <col min="45" max="45" width="28.140625" customWidth="1"/>
     <col min="46" max="47" width="28" customWidth="1"/>
-    <col min="48" max="48" width="27.85546875" customWidth="1"/>
-    <col min="49" max="49" width="28.140625" customWidth="1"/>
-    <col min="50" max="51" width="28" customWidth="1"/>
-    <col min="52" max="52" width="27.7109375" customWidth="1"/>
-    <col min="53" max="53" width="27.5703125" customWidth="1"/>
-    <col min="54" max="54" width="27.28515625" customWidth="1"/>
-    <col min="55" max="55" width="27.85546875" customWidth="1"/>
+    <col min="48" max="48" width="27.7109375" customWidth="1"/>
+    <col min="49" max="49" width="27.5703125" customWidth="1"/>
+    <col min="50" max="50" width="27.28515625" customWidth="1"/>
+    <col min="51" max="51" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:51" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -746,7 +655,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>8</v>
@@ -761,7 +670,7 @@
         <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>3</v>
@@ -776,10 +685,10 @@
         <v>0</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>12</v>
@@ -788,129 +697,117 @@
         <v>13</v>
       </c>
       <c r="R1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AM1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AN1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AO1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AO1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AP1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AR1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AS1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AT1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AU1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AV1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AW1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AX1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AY1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:51" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
         <v>46</v>
-      </c>
-      <c r="BA1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="BB1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="BC1" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:55" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="W2" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S1048576">
       <formula1>"Arpu, DIGI ZONE, IVAS, ON Mobil"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L420:O1048576">

</xml_diff>